<commit_message>
Feat: Now works with american stocks too.
</commit_message>
<xml_diff>
--- a/wallet.xlsx
+++ b/wallet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\Programas\Python\Projetos\Cotação de ações\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03090608-86CA-45CD-B2D7-AD6375C4B420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659C3A39-5E53-4FE7-9206-EE7E8A8896E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>PETR4.SA</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>ITUB3.SA</t>
+  </si>
+  <si>
+    <t>BBAS3.SA</t>
+  </si>
+  <si>
+    <t>AAPL</t>
   </si>
 </sst>
 </file>
@@ -368,7 +374,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,7 +403,15 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
       <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>

</xml_diff>